<commit_message>
Correction of data scale (divison by 1000) of acoustic data from visual experiment
</commit_message>
<xml_diff>
--- a/Data/Processed/07_Acoustic-Data_Visual-Exp.xlsx
+++ b/Data/Processed/07_Acoustic-Data_Visual-Exp.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Mestrado\Projeto\Artigos\Experimento\BESocio\Article_behav-S.max_V03\Data\Processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AC03BB-CE76-450F-A2BA-B18AE2699566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FD32EC-599E-4739-A329-B3B5E55EB4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="165" windowWidth="14520" windowHeight="10635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Call-frequency" sheetId="2" r:id="rId1"/>
     <sheet name="Emission-rate" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -403,10 +414,13 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -439,13 +453,13 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
       <c r="E2">
-        <v>2812500</v>
+        <v>2812.5</v>
       </c>
       <c r="F2">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -459,13 +473,13 @@
         <v>50</v>
       </c>
       <c r="D3">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
       <c r="E3">
-        <v>3187500</v>
+        <v>3187.5</v>
       </c>
       <c r="F3">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -479,13 +493,13 @@
         <v>50</v>
       </c>
       <c r="D4">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
       <c r="E4">
-        <v>3093750</v>
+        <v>3093.75</v>
       </c>
       <c r="F4">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -499,13 +513,13 @@
         <v>50</v>
       </c>
       <c r="D5">
-        <v>2156250</v>
+        <v>2156.25</v>
       </c>
       <c r="E5">
-        <v>2906250</v>
+        <v>2906.25</v>
       </c>
       <c r="F5">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -519,13 +533,13 @@
         <v>50</v>
       </c>
       <c r="D6">
-        <v>2156250</v>
+        <v>2156.25</v>
       </c>
       <c r="E6">
-        <v>3468750</v>
+        <v>3468.75</v>
       </c>
       <c r="F6">
-        <v>3468750</v>
+        <v>3468.75</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -539,13 +553,13 @@
         <v>50</v>
       </c>
       <c r="D7">
-        <v>2437500</v>
+        <v>2437.5</v>
       </c>
       <c r="E7">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="F7">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -559,13 +573,13 @@
         <v>50</v>
       </c>
       <c r="D8">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
       <c r="E8">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="F8">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -579,13 +593,13 @@
         <v>50</v>
       </c>
       <c r="D9">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
       <c r="E9">
-        <v>3187500</v>
+        <v>3187.5</v>
       </c>
       <c r="F9">
-        <v>2906250</v>
+        <v>2906.25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -599,13 +613,13 @@
         <v>50</v>
       </c>
       <c r="D10">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
       <c r="E10">
-        <v>3093750</v>
+        <v>3093.75</v>
       </c>
       <c r="F10">
-        <v>3093750</v>
+        <v>3093.75</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -619,13 +633,13 @@
         <v>50</v>
       </c>
       <c r="D11">
-        <v>2437500</v>
+        <v>2437.5</v>
       </c>
       <c r="E11">
-        <v>3093750</v>
+        <v>3093.75</v>
       </c>
       <c r="F11">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -639,13 +653,13 @@
         <v>50</v>
       </c>
       <c r="D12">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
       <c r="E12">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="F12">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -659,13 +673,13 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
       <c r="E13">
-        <v>3093750</v>
+        <v>3093.75</v>
       </c>
       <c r="F13">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -679,13 +693,13 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>2812500</v>
+        <v>2812.5</v>
       </c>
       <c r="E14">
-        <v>3187500</v>
+        <v>3187.5</v>
       </c>
       <c r="F14">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -699,13 +713,13 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>2437500</v>
+        <v>2437.5</v>
       </c>
       <c r="E15">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
       <c r="F15">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -719,13 +733,13 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
       <c r="E16">
-        <v>2906250</v>
+        <v>2906.25</v>
       </c>
       <c r="F16">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -739,13 +753,13 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
       <c r="E17">
-        <v>3093750</v>
+        <v>3093.75</v>
       </c>
       <c r="F17">
-        <v>3187500</v>
+        <v>3187.5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -759,13 +773,13 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
       <c r="E18">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="F18">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -779,13 +793,13 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
       <c r="E19">
-        <v>3187500</v>
+        <v>3187.5</v>
       </c>
       <c r="F19">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -799,13 +813,13 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>2437500</v>
+        <v>2437.5</v>
       </c>
       <c r="E20">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="F20">
-        <v>2343750</v>
+        <v>2343.75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -819,13 +833,13 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
       <c r="E21">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="F21">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -839,13 +853,13 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
       <c r="E22">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="F22">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -859,13 +873,13 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>6000000</v>
+        <v>6000</v>
       </c>
       <c r="E23">
-        <v>7781250</v>
+        <v>7781.25</v>
       </c>
       <c r="F23">
-        <v>6093750</v>
+        <v>6093.75</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -879,13 +893,13 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>2343750</v>
+        <v>2343.75</v>
       </c>
       <c r="E24">
-        <v>3281250</v>
+        <v>3281.25</v>
       </c>
       <c r="F24">
-        <v>2812500</v>
+        <v>2812.5</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -899,13 +913,13 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>2250000</v>
+        <v>2250</v>
       </c>
       <c r="E25">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="F25">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -919,13 +933,13 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>2250000</v>
+        <v>2250</v>
       </c>
       <c r="E26">
-        <v>3187500</v>
+        <v>3187.5</v>
       </c>
       <c r="F26">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -939,13 +953,13 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>2812500</v>
+        <v>2812.5</v>
       </c>
       <c r="E27">
-        <v>3093750</v>
+        <v>3093.75</v>
       </c>
       <c r="F27">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -959,13 +973,13 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
       <c r="E28">
-        <v>3093750</v>
+        <v>3093.75</v>
       </c>
       <c r="F28">
-        <v>2812500</v>
+        <v>2812.5</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -979,13 +993,13 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>2906250</v>
+        <v>2906.25</v>
       </c>
       <c r="E29">
-        <v>3468750</v>
+        <v>3468.75</v>
       </c>
       <c r="F29">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -999,13 +1013,13 @@
         <v>100</v>
       </c>
       <c r="D30">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
       <c r="E30">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="F30">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1019,13 +1033,13 @@
         <v>100</v>
       </c>
       <c r="D31">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
       <c r="E31">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="F31">
-        <v>2906250</v>
+        <v>2906.25</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,13 +1053,13 @@
         <v>100</v>
       </c>
       <c r="D32">
-        <v>2625000</v>
+        <v>2625</v>
       </c>
       <c r="E32">
-        <v>4687500</v>
+        <v>4687.5</v>
       </c>
       <c r="F32">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1059,13 +1073,13 @@
         <v>50</v>
       </c>
       <c r="D33">
-        <v>2812500</v>
+        <v>2812.5</v>
       </c>
       <c r="E33">
-        <v>5343750</v>
+        <v>5343.75</v>
       </c>
       <c r="F33">
-        <v>2812500</v>
+        <v>2812.5</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1079,13 +1093,13 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>2250000</v>
+        <v>2250</v>
       </c>
       <c r="E34">
-        <v>3750000</v>
+        <v>3750</v>
       </c>
       <c r="F34">
-        <v>2250000</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1099,13 +1113,13 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>2531250</v>
+        <v>2531.25</v>
       </c>
       <c r="E35">
-        <v>3468750</v>
+        <v>3468.75</v>
       </c>
       <c r="F35">
-        <v>2718750</v>
+        <v>2718.75</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1119,13 +1133,13 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <v>2250000</v>
+        <v>2250</v>
       </c>
       <c r="E36">
-        <v>3656250</v>
+        <v>3656.25</v>
       </c>
       <c r="F36">
-        <v>3281250</v>
+        <v>3281.25</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1139,13 +1153,13 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
       <c r="E37">
-        <v>3656250</v>
+        <v>3656.25</v>
       </c>
       <c r="F37">
-        <v>3000000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1159,13 +1173,13 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <v>2250000</v>
+        <v>2250</v>
       </c>
       <c r="E38">
-        <v>3562500</v>
+        <v>3562.5</v>
       </c>
       <c r="F38">
-        <v>3375000</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1179,13 +1193,13 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>2906250</v>
+        <v>2906.25</v>
       </c>
       <c r="E39">
-        <v>3843750</v>
+        <v>3843.75</v>
       </c>
       <c r="F39">
-        <v>3843750</v>
+        <v>3843.75</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1199,13 +1213,13 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>3093750</v>
+        <v>3093.75</v>
       </c>
       <c r="E40">
-        <v>3562500</v>
+        <v>3562.5</v>
       </c>
       <c r="F40">
-        <v>3281250</v>
+        <v>3281.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>